<commit_message>
Update docs for Lab5 for AVS
</commit_message>
<xml_diff>
--- a/AVS/Lab5/tabs_lab5_avs.xlsx
+++ b/AVS/Lab5/tabs_lab5_avs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
   <si>
     <t>1 Thread</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Boost 2000</t>
+  </si>
+  <si>
+    <t>8 Threads</t>
   </si>
 </sst>
 </file>
@@ -122,23 +125,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -420,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,24 +438,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="4"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -460,189 +464,207 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="3"/>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="3"/>
       <c r="J2" t="s">
         <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1.5880000000000001</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>3.11</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="3"/>
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>18.850000000000001</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>35.49</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="3"/>
       <c r="I3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>212.08600000000001</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <v>424.9</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1.042</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2.6869999999999998</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="3"/>
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>10.936999999999999</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>27.491</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="3"/>
       <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>133.369</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>345.875</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.77700000000000002</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2.5649999999999999</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>8.0220000000000002</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>24.555</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="3"/>
       <c r="I5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>104.84399999999999</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>319.46899999999999</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2.8959999999999999</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="10">
+        <v>7.9450000000000003</v>
+      </c>
+      <c r="G6" s="10">
+        <v>28.088999999999999</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2">
+        <v>106.79600000000001</v>
+      </c>
+      <c r="K6" s="10">
+        <v>410.27499999999998</v>
+      </c>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="4"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="1" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="4"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -651,43 +673,53 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="J10" t="s">
         <v>10</v>
       </c>
       <c r="K10" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>1.157</v>
+        <v>1.0509999999999999</v>
       </c>
       <c r="C11">
-        <v>1.212</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>1.101</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1.29</v>
+        <v>1.157</v>
       </c>
       <c r="G11">
-        <v>1.4450000000000001</v>
-      </c>
-      <c r="H11" s="4"/>
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1.1319999999999999</v>
+      </c>
       <c r="I11" t="s">
         <v>1</v>
       </c>
@@ -697,29 +729,35 @@
       <c r="K11">
         <v>1.33</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="10">
+        <v>1.036</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
-        <v>2.98</v>
+        <v>2.7</v>
       </c>
       <c r="C12">
-        <v>4.0030000000000001</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>3.63</v>
+      </c>
+      <c r="D12" s="10">
+        <v>4.22</v>
+      </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12">
-        <v>3.24</v>
+        <v>2.9089999999999998</v>
       </c>
       <c r="G12">
-        <v>4.42</v>
-      </c>
-      <c r="H12" s="4"/>
+        <v>3.96</v>
+      </c>
+      <c r="H12" s="10">
+        <v>3.9889999999999999</v>
+      </c>
       <c r="I12" t="s">
         <v>5</v>
       </c>
@@ -729,35 +767,37 @@
       <c r="K12">
         <v>4.0519999999999996</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="L12" s="10">
+        <v>3.98</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -783,22 +823,22 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>1.042</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>2.6869999999999998</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>10.936999999999999</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>27.491</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>133.369</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>345.875</v>
       </c>
     </row>
@@ -806,37 +846,60 @@
       <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.77700000000000002</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>2.5649999999999999</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>8.0220000000000002</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>24.555</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>104.84399999999999</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>319.46899999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2.8959999999999999</v>
+      </c>
+      <c r="D19" s="10">
+        <v>7.9450000000000003</v>
+      </c>
+      <c r="E19" s="10">
+        <v>28.088999999999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>106.79600000000001</v>
+      </c>
+      <c r="G19" s="10">
+        <v>410.27499999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A7:K7"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>